<commit_message>
rewards and armour added
</commit_message>
<xml_diff>
--- a/game_template/model/data/floor builder 20170212.xlsx
+++ b/game_template/model/data/floor builder 20170212.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8646" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8651" uniqueCount="247">
   <si>
     <t>width</t>
   </si>
@@ -492,21 +492,6 @@
         <family val="3"/>
       </rPr>
       <t>'Q'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">BOSS_DOOR = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF008080"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>'d'</t>
     </r>
   </si>
   <si>
@@ -1021,21 +1006,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">START_POSITON = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF008080"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>'='</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">SWITCH = </t>
     </r>
     <r>
@@ -1412,21 +1382,6 @@
         <family val="3"/>
       </rPr>
       <t>'¬'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>TILE1 = '`</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF008080"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>'</t>
     </r>
   </si>
   <si>
@@ -1942,6 +1897,216 @@
   <si>
     <t>F</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BOSS_DOOR = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'F'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BOSS_DOOR_OPEN = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'f'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DOOR_OPEN = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'d'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">REPLENISH = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"H"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BOSS = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'4'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BOSS_KEY = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'K'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PLAYER_ARMOUR = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'p'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PLAYER_GOLD = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'g'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PLAYER_SPIKE = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'A'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NPC1 = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'Y'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NPC2 = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'y'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">START_POSITION = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'='</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TILE1 = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'`'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">WALL3 = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'e'</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -2210,7 +2375,14 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="64">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3044,10 +3216,10 @@
         <v/>
       </c>
       <c r="AA1" s="15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AB1" s="15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="AF1">
         <f>LEN(AB1)</f>
@@ -3156,10 +3328,10 @@
         <v/>
       </c>
       <c r="AA2" s="15" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AB2" s="15" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF20" si="3">LEN(AB2)</f>
@@ -3268,10 +3440,10 @@
         <v/>
       </c>
       <c r="AA3" s="15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AB3" s="15" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AF3">
         <f t="shared" si="3"/>
@@ -3380,10 +3552,10 @@
         <v/>
       </c>
       <c r="AA4" s="15" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AB4" s="15" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AF4">
         <f t="shared" si="3"/>
@@ -3492,10 +3664,10 @@
         <v/>
       </c>
       <c r="AA5" s="15" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AB5" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="AF5">
         <f t="shared" si="3"/>
@@ -3604,10 +3776,10 @@
         <v/>
       </c>
       <c r="AA6" s="15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="AB6" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AF6">
         <f t="shared" si="3"/>
@@ -3716,10 +3888,10 @@
         <v/>
       </c>
       <c r="AA7" s="15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AB7" s="15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AF7">
         <f t="shared" si="3"/>
@@ -3828,10 +4000,10 @@
         <v/>
       </c>
       <c r="AA8" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="AB8" s="15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="AF8">
         <f t="shared" si="3"/>
@@ -3940,10 +4112,10 @@
         <v/>
       </c>
       <c r="AA9" s="15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="AB9" s="15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF9">
         <f t="shared" si="3"/>
@@ -4052,10 +4224,10 @@
         <v/>
       </c>
       <c r="AA10" s="15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="AB10" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AF10">
         <f t="shared" si="3"/>
@@ -4164,10 +4336,10 @@
         <v/>
       </c>
       <c r="AA11" s="15" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="AB11" s="15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF11">
         <f t="shared" si="3"/>
@@ -4276,10 +4448,10 @@
         <v/>
       </c>
       <c r="AA12" s="15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="AB12" s="15" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AF12">
         <f t="shared" si="3"/>
@@ -4388,10 +4560,10 @@
         <v/>
       </c>
       <c r="AA13" s="15" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="AB13" s="15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AF13">
         <f t="shared" si="3"/>
@@ -4500,10 +4672,10 @@
         <v/>
       </c>
       <c r="AA14" s="15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="AB14" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF14">
         <f t="shared" si="3"/>
@@ -4612,10 +4784,10 @@
         <v/>
       </c>
       <c r="AA15" s="15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AB15" s="15" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AF15">
         <f t="shared" si="3"/>
@@ -4724,10 +4896,10 @@
         <v/>
       </c>
       <c r="AA16" s="15" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AB16" s="15" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AF16">
         <f t="shared" si="3"/>
@@ -4836,10 +5008,10 @@
         <v/>
       </c>
       <c r="AA17" s="15" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="AB17" s="15" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AF17">
         <f t="shared" si="3"/>
@@ -4948,10 +5120,10 @@
         <v/>
       </c>
       <c r="AA18" s="15" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="AB18" s="15" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AF18">
         <f t="shared" si="3"/>
@@ -5060,10 +5232,10 @@
         <v/>
       </c>
       <c r="AA19" s="15" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="AB19" s="15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AF19">
         <f t="shared" si="3"/>
@@ -5172,10 +5344,10 @@
         <v/>
       </c>
       <c r="AA20" s="15" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="AB20" s="15" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="AF20">
         <f t="shared" si="3"/>
@@ -5345,12 +5517,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="62" priority="2">
+    <cfRule type="expression" dxfId="63" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="61" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7078,22 +7250,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="40" priority="4">
+    <cfRule type="expression" dxfId="41" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="39" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="38" priority="2">
+    <cfRule type="expression" dxfId="39" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="37" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8821,22 +8993,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="36" priority="4">
+    <cfRule type="expression" dxfId="37" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="35" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="34" priority="2">
+    <cfRule type="expression" dxfId="35" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="33" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9340,7 +9512,7 @@
         <v>2</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>2</v>
@@ -9415,7 +9587,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>2</v>
@@ -9490,7 +9662,7 @@
         <v>6</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>6</v>
@@ -9565,7 +9737,7 @@
         <v>6</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>6</v>
@@ -9640,7 +9812,7 @@
         <v>6</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>6</v>
@@ -10564,22 +10736,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="32" priority="4">
+    <cfRule type="expression" dxfId="33" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="31" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="30" priority="2">
+    <cfRule type="expression" dxfId="31" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11282,16 +11454,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>2</v>
@@ -11312,25 +11484,25 @@
         <v>6</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S10" s="14" t="s">
         <v>6</v>
@@ -11354,19 +11526,19 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>2</v>
@@ -11387,25 +11559,25 @@
         <v>6</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S11" s="14" t="s">
         <v>6</v>
@@ -12305,12 +12477,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13165,7 +13337,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>14</v>
@@ -13240,10 +13412,10 @@
         <v>22</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>7</v>
@@ -13315,7 +13487,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>12</v>
@@ -14038,12 +14210,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="25" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15771,12 +15943,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16454,13 +16626,13 @@
         <v>2</v>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T9" s="7" t="s">
         <v>2</v>
@@ -16490,13 +16662,13 @@
         <v>6</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>6</v>
@@ -16529,13 +16701,13 @@
         <v>2</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T10" s="7" t="s">
         <v>2</v>
@@ -16568,7 +16740,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>6</v>
@@ -16604,10 +16776,10 @@
         <v>8</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S11" s="14" t="s">
         <v>25</v>
@@ -16679,13 +16851,13 @@
         <v>2</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T12" s="7" t="s">
         <v>2</v>
@@ -17183,7 +17355,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K19" s="14" t="s">
         <v>2</v>
@@ -17507,12 +17679,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="22" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="21" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17941,13 +18113,13 @@
         <v>13</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>2</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M6" s="14" t="s">
         <v>14</v>
@@ -18016,13 +18188,13 @@
         <v>6</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>7</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M7" s="14" t="s">
         <v>6</v>
@@ -18091,13 +18263,13 @@
         <v>6</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>2</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M8" s="14" t="s">
         <v>6</v>
@@ -18142,10 +18314,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>6</v>
@@ -18193,10 +18365,10 @@
         <v>6</v>
       </c>
       <c r="S9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
@@ -18220,7 +18392,7 @@
         <v>110</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>6</v>
@@ -18268,7 +18440,7 @@
         <v>6</v>
       </c>
       <c r="S10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T10" s="7" t="s">
         <v>23</v>
@@ -18292,10 +18464,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>6</v>
@@ -18343,10 +18515,10 @@
         <v>6</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
@@ -18466,13 +18638,13 @@
         <v>6</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K13" s="14" t="s">
         <v>2</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M13" s="14" t="s">
         <v>6</v>
@@ -18541,13 +18713,13 @@
         <v>6</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>7</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M14" s="14" t="s">
         <v>6</v>
@@ -18616,13 +18788,13 @@
         <v>11</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K15" s="14" t="s">
         <v>2</v>
       </c>
       <c r="L15" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M15" s="14" t="s">
         <v>12</v>
@@ -19240,12 +19412,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="19" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19590,7 +19762,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H5" s="14" t="s">
         <v>16</v>
@@ -19665,10 +19837,10 @@
         <v>6</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>2</v>
@@ -20574,7 +20746,7 @@
         <v>6</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>6</v>
@@ -20646,13 +20818,13 @@
         <v>6</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L19" s="14" t="s">
         <v>6</v>
@@ -20718,19 +20890,19 @@
         <v>6</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J20" s="14" t="s">
         <v>18</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M20" s="14" t="s">
         <v>6</v>
@@ -20973,12 +21145,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21536,7 +21708,7 @@
         <v>110</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>2</v>
@@ -21608,10 +21780,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>2</v>
@@ -21683,10 +21855,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>2</v>
@@ -21728,13 +21900,13 @@
         <v>2</v>
       </c>
       <c r="Q10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T10" s="14" t="s">
         <v>2</v>
@@ -21779,7 +21951,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J11" s="14" t="s">
         <v>2</v>
@@ -21803,10 +21975,10 @@
         <v>31</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S11" s="14" t="s">
         <v>25</v>
@@ -21854,7 +22026,7 @@
         <v>9</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J12" s="14" t="s">
         <v>9</v>
@@ -21881,10 +22053,10 @@
         <v>31</v>
       </c>
       <c r="R12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T12" s="14" t="s">
         <v>2</v>
@@ -22706,12 +22878,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="15" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24439,12 +24611,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="60" priority="2">
+    <cfRule type="expression" dxfId="61" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="59" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25148,10 +25320,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>2</v>
@@ -25223,13 +25395,13 @@
         <v>22</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E11" s="14">
         <v>8</v>
@@ -25274,7 +25446,7 @@
         <v>8</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T11" s="14" t="s">
         <v>23</v>
@@ -25298,10 +25470,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>2</v>
@@ -26231,22 +26403,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22:Y25 U21:Y21 A1:Y20">
-    <cfRule type="expression" dxfId="14" priority="4">
+    <cfRule type="expression" dxfId="15" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:Z25 U21:Z21 A1:Z20">
-    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26260,7 +26432,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U20"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26376,13 +26548,13 @@
         <v>2</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>25</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="L2" s="14" t="s">
         <v>2</v>
@@ -26422,11 +26594,11 @@
       </c>
       <c r="AA2" t="str">
         <f t="shared" ref="AA2:AA25" si="1">CONCATENATE(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2,R2,S2,T2,U2,V2,W2,X2,Y2)</f>
-        <v>:)     : j :      (:</v>
+        <v>:)     :`j`:      (:</v>
       </c>
       <c r="AB2" t="str">
         <f t="shared" ref="AB2:AB25" si="2">"'"&amp;AA2&amp;"',"</f>
-        <v>':)     : j :      (:',</v>
+        <v>':)     :`j`:      (:',</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -26455,13 +26627,13 @@
         <v>2</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="L3" s="14" t="s">
         <v>2</v>
@@ -26501,11 +26673,11 @@
       </c>
       <c r="AA3" t="str">
         <f t="shared" si="1"/>
-        <v>:      :   :       :</v>
+        <v>:      :```:       :</v>
       </c>
       <c r="AB3" t="str">
         <f t="shared" si="2"/>
-        <v>':      :   :       :',</v>
+        <v>':      :```:       :',</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -26612,14 +26784,14 @@
       <c r="H5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>6</v>
+      <c r="I5" s="14">
+        <v>8</v>
+      </c>
+      <c r="J5" s="14">
+        <v>8</v>
+      </c>
+      <c r="K5" s="14">
+        <v>8</v>
       </c>
       <c r="L5" s="14" t="s">
         <v>6</v>
@@ -26659,11 +26831,11 @@
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="1"/>
-        <v>:                  :</v>
+        <v>:       888        :</v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="2"/>
-        <v>':                  :',</v>
+        <v>':       888        :',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -26841,13 +27013,13 @@
         <v>2</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>6</v>
@@ -26908,31 +27080,31 @@
         <v>2</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>6</v>
@@ -26987,34 +27159,34 @@
         <v>2</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L10" s="14" t="s">
         <v>6</v>
@@ -27066,58 +27238,58 @@
         <v>2</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T11" s="7" t="s">
         <v>23</v>
@@ -27145,34 +27317,34 @@
         <v>2</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L12" s="14" t="s">
         <v>6</v>
@@ -27224,31 +27396,31 @@
         <v>2</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K13" s="14" t="s">
         <v>6</v>
@@ -27315,13 +27487,13 @@
         <v>2</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I14" s="14" t="s">
         <v>6</v>
@@ -27481,14 +27653,14 @@
       <c r="H16" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>6</v>
+      <c r="I16" s="14">
+        <v>8</v>
+      </c>
+      <c r="J16" s="14">
+        <v>8</v>
+      </c>
+      <c r="K16" s="14">
+        <v>8</v>
       </c>
       <c r="L16" s="14" t="s">
         <v>6</v>
@@ -27528,11 +27700,11 @@
       </c>
       <c r="AA16" t="str">
         <f t="shared" si="1"/>
-        <v>:x                 :</v>
+        <v>:x      888        :</v>
       </c>
       <c r="AB16" t="str">
         <f t="shared" si="2"/>
-        <v>':x                 :',</v>
+        <v>':x      888        :',</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -27640,13 +27812,13 @@
         <v>2</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="L18" s="14" t="s">
         <v>2</v>
@@ -27686,11 +27858,11 @@
       </c>
       <c r="AA18" t="str">
         <f t="shared" si="1"/>
-        <v>:      :   :       :</v>
+        <v>:      :```:       :</v>
       </c>
       <c r="AB18" t="str">
         <f t="shared" si="2"/>
-        <v>':      :   :       :',</v>
+        <v>':      :```:       :',</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -27719,13 +27891,13 @@
         <v>2</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>25</v>
+        <v>194</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="L19" s="14" t="s">
         <v>2</v>
@@ -27765,11 +27937,11 @@
       </c>
       <c r="AA19" t="str">
         <f t="shared" si="1"/>
-        <v>:\     : j :      /:</v>
+        <v>:\     :```:      /:</v>
       </c>
       <c r="AB19" t="str">
         <f t="shared" si="2"/>
-        <v>':\     : j :      /:',</v>
+        <v>':\     :```:      /:',</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -28114,17 +28286,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z20">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28570,13 +28742,13 @@
         <v>6</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L6" s="14" t="s">
         <v>6</v>
@@ -28649,13 +28821,13 @@
         <v>6</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L7" s="14" t="s">
         <v>6</v>
@@ -28728,13 +28900,13 @@
         <v>6</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L8" s="14" t="s">
         <v>6</v>
@@ -28807,13 +28979,13 @@
         <v>6</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L9" s="14" t="s">
         <v>6</v>
@@ -28886,13 +29058,13 @@
         <v>6</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L10" s="14" t="s">
         <v>6</v>
@@ -28965,13 +29137,13 @@
         <v>6</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L11" s="14" t="s">
         <v>6</v>
@@ -29044,13 +29216,13 @@
         <v>6</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L12" s="14" t="s">
         <v>6</v>
@@ -29123,13 +29295,13 @@
         <v>6</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L13" s="14" t="s">
         <v>6</v>
@@ -29202,13 +29374,13 @@
         <v>6</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L14" s="14" t="s">
         <v>6</v>
@@ -29281,13 +29453,13 @@
         <v>6</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L15" s="14" t="s">
         <v>6</v>
@@ -29363,7 +29535,7 @@
         <v>6</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K16" s="14" t="s">
         <v>6</v>
@@ -29442,7 +29614,7 @@
         <v>6</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K17" s="14" t="s">
         <v>6</v>
@@ -29992,32 +30164,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y20 A22:Y25 U21:Y21">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y20 A22:Z25 U21:Z21">
-    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:T21">
-    <cfRule type="cellIs" dxfId="4" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z20">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z1:Z20">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30028,11 +30200,11 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30116,15 +30288,15 @@
         <v>BEACH ='b'</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>196</v>
+        <v>134</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I65" si="2">TRIM(MID($H3,1,FIND("=",$H3)-1))</f>
-        <v>TILE1</v>
+        <f t="shared" ref="I3:I66" si="2">TRIM(MID($H3,1,FIND("=",$H3)-1))</f>
+        <v>BOMB</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J65" si="3">SUBSTITUTE(TRIM(MID($H3,FIND("=",$H3)+1,200)),"'","")</f>
-        <v>`</v>
+        <f t="shared" ref="J3:J66" si="3">SUBSTITUTE(TRIM(MID($H3,FIND("=",$H3)+1,200)),"'","")</f>
+        <v>q</v>
       </c>
       <c r="K3" s="20" t="b">
         <f t="shared" ref="K3:K65" si="4">SUMPRODUCT(--(EXACT(J:J,J3)))&gt;1</f>
@@ -30147,15 +30319,15 @@
         <v>BOMB ='q'</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>195</v>
+        <v>135</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="2"/>
-        <v>TILE2</v>
+        <v>BOMB_LIT</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="3"/>
-        <v>¬</v>
+        <v>Q</v>
       </c>
       <c r="K4" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30178,15 +30350,15 @@
         <v>BOMB_LIT ='Q'</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>193</v>
+        <v>233</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="2"/>
-        <v>TILE3</v>
+        <v>BOSS_DOOR</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="3"/>
-        <v>.</v>
+        <v>F</v>
       </c>
       <c r="K5" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30209,15 +30381,15 @@
         <v>BOSS_DOOR ='d'</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>194</v>
+        <v>234</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="2"/>
-        <v>TILE4</v>
+        <v>BOSS_DOOR_OPEN</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="3"/>
-        <v>~</v>
+        <v>f</v>
       </c>
       <c r="K6" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30240,15 +30412,15 @@
         <v>BRAZIER ='B'</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="2"/>
-        <v>BOMB</v>
+        <v>BRAZIER</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="3"/>
-        <v>q</v>
+        <v>B</v>
       </c>
       <c r="K7" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30271,15 +30443,15 @@
         <v>CLOUD ='.'</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="2"/>
-        <v>BOMB_LIT</v>
+        <v>DECORATION1</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="3"/>
-        <v>Q</v>
+        <v>z</v>
       </c>
       <c r="K8" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30302,15 +30474,15 @@
         <v>DECORATION1 ='z'</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="2"/>
-        <v>BOSS_DOOR</v>
+        <v>DECORATION2</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="3"/>
-        <v>d</v>
+        <v>Z</v>
       </c>
       <c r="K9" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30333,15 +30505,15 @@
         <v>DECORATION2 ='Z'</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="2"/>
-        <v>BRAZIER</v>
+        <v>DOOR</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="3"/>
-        <v>B</v>
+        <v>D</v>
       </c>
       <c r="K10" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30364,15 +30536,15 @@
         <v>DOOR ='D'</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>138</v>
+        <v>235</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="2"/>
-        <v>DECORATION1</v>
+        <v>DOOR_OPEN</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="3"/>
-        <v>z</v>
+        <v>d</v>
       </c>
       <c r="K11" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30395,15 +30567,15 @@
         <v>DOT1 ='!'</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="2"/>
-        <v>DECORATION2</v>
+        <v>DOT1</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="3"/>
-        <v>Z</v>
+        <v>!</v>
       </c>
       <c r="K12" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30426,15 +30598,15 @@
         <v>DOT2 ='£'</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="2"/>
-        <v>DOOR</v>
+        <v>DOT2</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="3"/>
-        <v>D</v>
+        <v>£</v>
       </c>
       <c r="K13" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30457,15 +30629,15 @@
         <v>DOWN ='-'</v>
       </c>
       <c r="H14" s="28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="2"/>
-        <v>DOT1</v>
+        <v>DOWN</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="3"/>
-        <v>!</v>
+        <v>-</v>
       </c>
       <c r="K14" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30488,15 +30660,15 @@
         <v>EAST ='E'</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="2"/>
-        <v>DOT2</v>
+        <v>EAST</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="3"/>
-        <v>£</v>
+        <v>E</v>
       </c>
       <c r="K15" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30519,15 +30691,15 @@
         <v>EMPTY =' '</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="2"/>
-        <v>DOWN</v>
+        <v>EMPTY</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="K16" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30550,15 +30722,15 @@
         <v>EXIT_KEY ='%'</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="2"/>
-        <v>EAST</v>
+        <v>EXIT_KEY</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="3"/>
-        <v>E</v>
+        <v>%</v>
       </c>
       <c r="K17" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30581,15 +30753,15 @@
         <v>HEART ='HP'</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="2"/>
-        <v>EMPTY</v>
+        <v>HEART</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
+        <v>HP</v>
       </c>
       <c r="K18" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30612,15 +30784,15 @@
         <v>KEY ='?'</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>146</v>
+        <v>236</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="2"/>
-        <v>EXIT_KEY</v>
+        <v>REPLENISH</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="3"/>
-        <v>%</v>
+        <v>"H"</v>
       </c>
       <c r="K19" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30647,11 +30819,11 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" si="2"/>
-        <v>HEART</v>
+        <v>KEY</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="3"/>
-        <v>HP</v>
+        <v>?</v>
       </c>
       <c r="K20" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30678,11 +30850,11 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="2"/>
-        <v>KEY</v>
+        <v>MAP</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="3"/>
-        <v>?</v>
+        <v>M</v>
       </c>
       <c r="K21" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30709,11 +30881,11 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" si="2"/>
-        <v>MAP</v>
+        <v>MONSTER1</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="3"/>
-        <v>M</v>
+        <v>1</v>
       </c>
       <c r="K22" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30740,11 +30912,11 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" si="2"/>
-        <v>MONSTER1</v>
+        <v>MONSTER2</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K23" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30771,11 +30943,11 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" si="2"/>
-        <v>MONSTER2</v>
+        <v>MONSTER3</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K24" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30798,15 +30970,15 @@
         <v>NORTH ='N'</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>152</v>
+        <v>237</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="2"/>
-        <v>MONSTER3</v>
+        <v>BOSS</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K25" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30829,15 +31001,15 @@
         <v>PLAYER ='P'</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>153</v>
+        <v>238</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="2"/>
-        <v>NEXT_LEVEL</v>
+        <v>BOSS_KEY</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="3"/>
-        <v>L</v>
+        <v>K</v>
       </c>
       <c r="K26" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30860,15 +31032,15 @@
         <v>PREVIOUS_LEVEL ='l'</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="2"/>
-        <v>NORTH</v>
+        <v>NEXT_LEVEL</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="3"/>
-        <v>N</v>
+        <v>L</v>
       </c>
       <c r="K27" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30891,15 +31063,15 @@
         <v>RED_POTION ='R'</v>
       </c>
       <c r="H28" s="28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="2"/>
-        <v>PLAYER</v>
+        <v>NORTH</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="3"/>
-        <v>P</v>
+        <v>N</v>
       </c>
       <c r="K28" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30922,15 +31094,15 @@
         <v>RUNE ='u'</v>
       </c>
       <c r="H29" s="28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="2"/>
-        <v>PREVIOUS_LEVEL</v>
+        <v>PLAYER</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="3"/>
-        <v>l</v>
+        <v>P</v>
       </c>
       <c r="K29" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30953,15 +31125,15 @@
         <v>RUNE1 ='R1'</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="2"/>
-        <v>RED_POTION</v>
+        <v>PLAYER_ARMOUR</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="3"/>
-        <v>R</v>
+        <v>p</v>
       </c>
       <c r="K30" s="20" t="b">
         <f t="shared" si="4"/>
@@ -30984,15 +31156,15 @@
         <v>RUNE2 ='R2'</v>
       </c>
       <c r="H31" s="28" t="s">
-        <v>158</v>
+        <v>240</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="2"/>
-        <v>RUNE</v>
+        <v>PLAYER_GOLD</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="3"/>
-        <v>u</v>
+        <v>g</v>
       </c>
       <c r="K31" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31015,15 +31187,15 @@
         <v>RUNE3 ='R3'</v>
       </c>
       <c r="H32" s="28" t="s">
-        <v>159</v>
+        <v>241</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="2"/>
-        <v>RUNE1</v>
+        <v>PLAYER_SPIKE</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="3"/>
-        <v>R1</v>
+        <v>A</v>
       </c>
       <c r="K32" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31046,15 +31218,15 @@
         <v>RUNE4 ='R4'</v>
       </c>
       <c r="H33" s="28" t="s">
-        <v>160</v>
+        <v>242</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="2"/>
-        <v>RUNE2</v>
+        <v>NPC1</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="3"/>
-        <v>R2</v>
+        <v>Y</v>
       </c>
       <c r="K33" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31077,15 +31249,15 @@
         <v>RUNE5 ='R5'</v>
       </c>
       <c r="H34" s="28" t="s">
-        <v>161</v>
+        <v>243</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="2"/>
-        <v>RUNE3</v>
+        <v>NPC2</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="3"/>
-        <v>R3</v>
+        <v>y</v>
       </c>
       <c r="K34" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31108,15 +31280,15 @@
         <v>SAFETY ='8'</v>
       </c>
       <c r="H35" s="28" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="2"/>
-        <v>RUNE4</v>
+        <v>PREVIOUS_LEVEL</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="3"/>
-        <v>R4</v>
+        <v>l</v>
       </c>
       <c r="K35" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31139,15 +31311,15 @@
         <v>SECRET_TREASURE ='J'</v>
       </c>
       <c r="H36" s="28" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="2"/>
-        <v>RUNE5</v>
+        <v>RED_POTION</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="3"/>
-        <v>R5</v>
+        <v>R</v>
       </c>
       <c r="K36" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31170,15 +31342,15 @@
         <v>SECRET_WALL =';'</v>
       </c>
       <c r="H37" s="28" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" si="2"/>
-        <v>SAFETY</v>
+        <v>RUNE</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>u</v>
       </c>
       <c r="K37" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31201,15 +31373,15 @@
         <v>SHIELD ='O'</v>
       </c>
       <c r="H38" s="28" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="I38" t="str">
         <f t="shared" si="2"/>
-        <v>SECRET_TREASURE</v>
+        <v>RUNE1</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="3"/>
-        <v>J</v>
+        <v>R1</v>
       </c>
       <c r="K38" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31232,15 +31404,15 @@
         <v>SHOP ='s'</v>
       </c>
       <c r="H39" s="28" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="2"/>
-        <v>SECRET_WALL</v>
+        <v>RUNE2</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="3"/>
-        <v>;</v>
+        <v>R2</v>
       </c>
       <c r="K39" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31263,15 +31435,15 @@
         <v>SHOP_KEEPER ='SHOP'</v>
       </c>
       <c r="H40" s="28" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="2"/>
-        <v>SHIELD</v>
+        <v>RUNE3</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" si="3"/>
-        <v>O</v>
+        <v>R3</v>
       </c>
       <c r="K40" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31294,15 +31466,15 @@
         <v>SKY ='~'</v>
       </c>
       <c r="H41" s="28" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="2"/>
-        <v>SHOP</v>
+        <v>RUNE4</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="3"/>
-        <v>s</v>
+        <v>R4</v>
       </c>
       <c r="K41" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31325,15 +31497,15 @@
         <v>SOUTH ='S'</v>
       </c>
       <c r="H42" s="28" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="2"/>
-        <v>SHOP_KEEPER</v>
+        <v>RUNE5</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="3"/>
-        <v>SHOP</v>
+        <v>R5</v>
       </c>
       <c r="K42" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31356,15 +31528,15 @@
         <v>START_POSITON ='='</v>
       </c>
       <c r="H43" s="28" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="2"/>
-        <v>SOUTH</v>
+        <v>SAFETY</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="3"/>
-        <v>S</v>
+        <v>8</v>
       </c>
       <c r="K43" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31387,15 +31559,15 @@
         <v>SWITCH =','</v>
       </c>
       <c r="H44" s="28" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="I44" t="str">
         <f t="shared" si="2"/>
-        <v>START_POSITON</v>
+        <v>SECRET_TREASURE</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="3"/>
-        <v>=</v>
+        <v>J</v>
       </c>
       <c r="K44" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31418,15 +31590,15 @@
         <v>SWITCH_LIT ='&lt;'</v>
       </c>
       <c r="H45" s="28" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="2"/>
-        <v>SWITCH</v>
+        <v>SECRET_WALL</v>
       </c>
       <c r="J45" t="str">
         <f t="shared" si="3"/>
-        <v>,</v>
+        <v>;</v>
       </c>
       <c r="K45" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31449,15 +31621,15 @@
         <v>SWITCH_TILE ='_'</v>
       </c>
       <c r="H46" s="28" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="I46" t="str">
         <f t="shared" si="2"/>
-        <v>SWITCH_LIT</v>
+        <v>SHIELD</v>
       </c>
       <c r="J46" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;</v>
+        <v>O</v>
       </c>
       <c r="K46" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31480,15 +31652,15 @@
         <v>TRAP1 ='^'</v>
       </c>
       <c r="H47" s="28" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="2"/>
-        <v>SWITCH_TILE</v>
+        <v>SHOP</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="3"/>
-        <v>_</v>
+        <v>s</v>
       </c>
       <c r="K47" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31511,15 +31683,15 @@
         <v>TRAP2 ='&amp;'</v>
       </c>
       <c r="H48" s="28" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="2"/>
-        <v>TRAP1</v>
+        <v>SHOP_KEEPER</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="3"/>
-        <v>^</v>
+        <v>SHOP</v>
       </c>
       <c r="K48" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31542,15 +31714,15 @@
         <v>TRAP3 ='['</v>
       </c>
       <c r="H49" s="28" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="I49" t="str">
         <f t="shared" si="2"/>
-        <v>TRAP2</v>
+        <v>SOUTH</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="3"/>
-        <v>&amp;</v>
+        <v>S</v>
       </c>
       <c r="K49" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31573,15 +31745,15 @@
         <v>TREASURE ='*'</v>
       </c>
       <c r="H50" s="28" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="I50" t="str">
         <f t="shared" si="2"/>
-        <v>TRAP3</v>
+        <v>START_POSITION</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="3"/>
-        <v>[</v>
+        <v>=</v>
       </c>
       <c r="K50" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31604,15 +31776,15 @@
         <v>TREASURE_CHEST ='j'</v>
       </c>
       <c r="H51" s="28" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="2"/>
-        <v>TREASURE</v>
+        <v>SWITCH</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" si="3"/>
-        <v>*</v>
+        <v>,</v>
       </c>
       <c r="K51" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31635,15 +31807,15 @@
         <v>TREASURE10 ='x'</v>
       </c>
       <c r="H52" s="28" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="2"/>
-        <v>TREASURE_CHEST</v>
+        <v>SWITCH_LIT</v>
       </c>
       <c r="J52" t="str">
         <f t="shared" si="3"/>
-        <v>j</v>
+        <v>&lt;</v>
       </c>
       <c r="K52" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31666,15 +31838,15 @@
         <v>TREASURE25 ='X'</v>
       </c>
       <c r="H53" s="28" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="2"/>
-        <v>TREASURE10</v>
+        <v>SWITCH_TILE</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="3"/>
-        <v>x</v>
+        <v>_</v>
       </c>
       <c r="K53" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31697,15 +31869,15 @@
         <v>TREE ='T'</v>
       </c>
       <c r="H54" s="28" t="s">
-        <v>181</v>
+        <v>245</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="2"/>
-        <v>TREASURE25</v>
+        <v>TILE1</v>
       </c>
       <c r="J54" t="str">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>`</v>
       </c>
       <c r="K54" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31728,15 +31900,15 @@
         <v>TROPHY ='G'</v>
       </c>
       <c r="H55" s="28" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="2"/>
-        <v>TREE</v>
+        <v>TILE2</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>¬</v>
       </c>
       <c r="K55" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31759,15 +31931,15 @@
         <v>UP ='+'</v>
       </c>
       <c r="H56" s="28" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="I56" t="str">
         <f t="shared" si="2"/>
-        <v>TROPHY</v>
+        <v>TILE3</v>
       </c>
       <c r="J56" t="str">
         <f t="shared" si="3"/>
-        <v>G</v>
+        <v>.</v>
       </c>
       <c r="K56" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31790,15 +31962,15 @@
         <v>WALL =':'</v>
       </c>
       <c r="H57" s="28" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="2"/>
-        <v>UP</v>
+        <v>TILE4</v>
       </c>
       <c r="J57" t="str">
         <f t="shared" si="3"/>
-        <v>+</v>
+        <v>~</v>
       </c>
       <c r="K57" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31821,15 +31993,15 @@
         <v>WALL_BL ='('</v>
       </c>
       <c r="H58" s="28" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" si="2"/>
-        <v>WALL</v>
+        <v>TRAP1</v>
       </c>
       <c r="J58" t="str">
         <f t="shared" si="3"/>
-        <v>:</v>
+        <v>^</v>
       </c>
       <c r="K58" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31852,15 +32024,15 @@
         <v>WALL_BR =')'</v>
       </c>
       <c r="H59" s="28" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="I59" t="str">
         <f t="shared" si="2"/>
-        <v>WALL_BL</v>
+        <v>TRAP2</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" si="3"/>
-        <v>(</v>
+        <v>&amp;</v>
       </c>
       <c r="K59" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31883,15 +32055,15 @@
         <v>WALL_TL ='/'</v>
       </c>
       <c r="H60" s="28" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="I60" t="str">
         <f t="shared" si="2"/>
-        <v>WALL_BR</v>
+        <v>TRAP3</v>
       </c>
       <c r="J60" t="str">
         <f t="shared" si="3"/>
-        <v>)</v>
+        <v>[</v>
       </c>
       <c r="K60" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31914,15 +32086,15 @@
         <v>WALL_TR ='\\'</v>
       </c>
       <c r="H61" s="28" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="I61" t="str">
         <f t="shared" si="2"/>
-        <v>WALL_TL</v>
+        <v>TREASURE</v>
       </c>
       <c r="J61" t="str">
         <f t="shared" si="3"/>
-        <v>/</v>
+        <v>*</v>
       </c>
       <c r="K61" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31945,15 +32117,15 @@
         <v>WATER ='w'</v>
       </c>
       <c r="H62" s="28" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="I62" t="str">
         <f t="shared" si="2"/>
-        <v>WALL_TR</v>
+        <v>TREASURE_CHEST</v>
       </c>
       <c r="J62" t="str">
         <f t="shared" si="3"/>
-        <v>\\</v>
+        <v>j</v>
       </c>
       <c r="K62" s="20" t="b">
         <f t="shared" si="4"/>
@@ -31976,15 +32148,15 @@
         <v>WEAPON ='|'</v>
       </c>
       <c r="H63" s="28" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="I63" t="str">
         <f t="shared" si="2"/>
-        <v>WALL2</v>
+        <v>TREASURE10</v>
       </c>
       <c r="J63" t="str">
         <f t="shared" si="3"/>
-        <v>w</v>
+        <v>x</v>
       </c>
       <c r="K63" s="20" t="b">
         <f t="shared" si="4"/>
@@ -32007,15 +32179,15 @@
         <v>WEST ='W'</v>
       </c>
       <c r="H64" s="28" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="I64" t="str">
         <f t="shared" si="2"/>
-        <v>WEAPON</v>
+        <v>TREASURE25</v>
       </c>
       <c r="J64" t="str">
         <f t="shared" si="3"/>
-        <v>|</v>
+        <v>X</v>
       </c>
       <c r="K64" s="20" t="b">
         <f t="shared" si="4"/>
@@ -32024,18 +32196,205 @@
     </row>
     <row r="65" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H65" s="28" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="I65" t="str">
         <f t="shared" si="2"/>
-        <v>WEST</v>
+        <v>TREE</v>
       </c>
       <c r="J65" t="str">
         <f t="shared" si="3"/>
-        <v>W</v>
+        <v>T</v>
       </c>
       <c r="K65" s="20" t="b">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H66" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="2"/>
+        <v>TROPHY</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="3"/>
+        <v>G</v>
+      </c>
+      <c r="K66" s="20" t="b">
+        <f t="shared" ref="K66:K76" si="6">SUMPRODUCT(--(EXACT(J:J,J66)))&gt;1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H67" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" ref="I67:I76" si="7">TRIM(MID($H67,1,FIND("=",$H67)-1))</f>
+        <v>UP</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" ref="J67:J76" si="8">SUBSTITUTE(TRIM(MID($H67,FIND("=",$H67)+1,200)),"'","")</f>
+        <v>+</v>
+      </c>
+      <c r="K67" s="20" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H68" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="7"/>
+        <v>WALL</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" si="8"/>
+        <v>:</v>
+      </c>
+      <c r="K68" s="20" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H69" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="7"/>
+        <v>WALL_BL</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="8"/>
+        <v>(</v>
+      </c>
+      <c r="K69" s="20" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H70" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="I70" t="str">
+        <f t="shared" si="7"/>
+        <v>WALL_BR</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="8"/>
+        <v>)</v>
+      </c>
+      <c r="K70" s="20" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H71" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" si="7"/>
+        <v>WALL_TL</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="8"/>
+        <v>/</v>
+      </c>
+      <c r="K71" s="20" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H72" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="I72" t="str">
+        <f t="shared" si="7"/>
+        <v>WALL_TR</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="8"/>
+        <v>\\</v>
+      </c>
+      <c r="K72" s="20" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H73" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="I73" t="str">
+        <f t="shared" si="7"/>
+        <v>WALL2</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="8"/>
+        <v>w</v>
+      </c>
+      <c r="K73" s="20" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H74" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="I74" t="str">
+        <f t="shared" si="7"/>
+        <v>WALL3</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="8"/>
+        <v>e</v>
+      </c>
+      <c r="K74" s="20" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H75" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" si="7"/>
+        <v>WEAPON</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" si="8"/>
+        <v>|</v>
+      </c>
+      <c r="K75" s="20" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H76" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="I76" t="str">
+        <f t="shared" si="7"/>
+        <v>WEST</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="8"/>
+        <v>W</v>
+      </c>
+      <c r="K76" s="20" t="b">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -32045,12 +32404,12 @@
     <sortCondition ref="B2:B67"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K65">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="K2:K76">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33778,12 +34137,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="58" priority="2">
+    <cfRule type="expression" dxfId="59" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="57" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33912,7 +34271,7 @@
         <v>6</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>6</v>
@@ -33987,7 +34346,7 @@
         <v>6</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>6</v>
@@ -34062,7 +34421,7 @@
         <v>10</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K4" s="14" t="s">
         <v>6</v>
@@ -34137,7 +34496,7 @@
         <v>6</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>6</v>
@@ -34212,7 +34571,7 @@
         <v>6</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>6</v>
@@ -34287,7 +34646,7 @@
         <v>105</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>6</v>
@@ -34338,31 +34697,31 @@
         <v>22</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>6</v>
@@ -34437,7 +34796,7 @@
         <v>6</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>6</v>
@@ -34509,13 +34868,13 @@
         <v>6</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L10" s="14" t="s">
         <v>6</v>
@@ -34584,37 +34943,37 @@
         <v>6</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J11" s="14" t="s">
         <v>19</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="Q11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T11" s="14" t="s">
         <v>23</v>
@@ -34659,19 +35018,19 @@
         <v>6</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L12" s="14" t="s">
         <v>6</v>
       </c>
       <c r="M12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N12" s="14" t="s">
         <v>105</v>
@@ -34748,7 +35107,7 @@
         <v>6</v>
       </c>
       <c r="M13" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N13" s="14" t="s">
         <v>6</v>
@@ -34823,7 +35182,7 @@
         <v>6</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N14" s="14" t="s">
         <v>6</v>
@@ -34898,7 +35257,7 @@
         <v>6</v>
       </c>
       <c r="M15" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N15" s="14" t="s">
         <v>6</v>
@@ -34949,7 +35308,7 @@
         <v>9</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>9</v>
@@ -34973,7 +35332,7 @@
         <v>6</v>
       </c>
       <c r="M16" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N16" s="14" t="s">
         <v>6</v>
@@ -35024,7 +35383,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F17" s="14">
         <v>8</v>
@@ -35048,7 +35407,7 @@
         <v>6</v>
       </c>
       <c r="M17" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N17" s="14" t="s">
         <v>10</v>
@@ -35099,31 +35458,31 @@
         <v>6</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N18" s="14" t="s">
         <v>6</v>
@@ -35189,7 +35548,7 @@
         <v>6</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K19" s="14" t="s">
         <v>6</v>
@@ -35513,22 +35872,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y13 A18:Y25 A14:C17 G14:Y17">
-    <cfRule type="expression" dxfId="56" priority="4">
+    <cfRule type="expression" dxfId="57" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z13 A18:Z25 A14:C17 G14:Z17">
-    <cfRule type="cellIs" dxfId="55" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:F17">
-    <cfRule type="expression" dxfId="54" priority="2">
+    <cfRule type="expression" dxfId="55" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:F17">
-    <cfRule type="cellIs" dxfId="53" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36257,7 +36616,7 @@
         <v>6</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>6</v>
@@ -36329,13 +36688,13 @@
         <v>6</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J11" s="14" t="s">
         <v>16</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L11" s="14" t="s">
         <v>6</v>
@@ -36407,7 +36766,7 @@
         <v>6</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K12" s="14" t="s">
         <v>6</v>
@@ -37256,12 +37615,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="52" priority="2">
+    <cfRule type="expression" dxfId="53" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="51" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37390,7 +37749,7 @@
         <v>2</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>2</v>
@@ -37465,7 +37824,7 @@
         <v>2</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K3" s="14" t="s">
         <v>2</v>
@@ -38089,7 +38448,7 @@
         <v>15</v>
       </c>
       <c r="R11" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S11" s="14" t="s">
         <v>8</v>
@@ -38140,7 +38499,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K12" s="14" t="s">
         <v>2</v>
@@ -38590,7 +38949,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K18" s="14" t="s">
         <v>2</v>
@@ -38989,12 +39348,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="50" priority="2">
+    <cfRule type="expression" dxfId="51" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="49" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39699,7 +40058,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>7</v>
@@ -40302,7 +40661,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>2</v>
@@ -40347,7 +40706,7 @@
         <v>2</v>
       </c>
       <c r="R18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S18" s="14" t="s">
         <v>2</v>
@@ -40377,7 +40736,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>2</v>
@@ -40422,7 +40781,7 @@
         <v>2</v>
       </c>
       <c r="R19" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S19" s="14" t="s">
         <v>25</v>
@@ -40814,12 +41173,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y26">
-    <cfRule type="expression" dxfId="48" priority="2">
+    <cfRule type="expression" dxfId="49" priority="2">
       <formula>AND(COLUMN()&lt;=$B$27,ROW()&lt;=$B$28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z26">
-    <cfRule type="cellIs" dxfId="47" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41533,10 +41892,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>2</v>
@@ -41608,10 +41967,10 @@
         <v>8</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>7</v>
@@ -41683,10 +42042,10 @@
         <v>6</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>2</v>
@@ -42547,22 +42906,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="46" priority="4">
+    <cfRule type="expression" dxfId="47" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="45" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="44" priority="2">
+    <cfRule type="expression" dxfId="45" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="43" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42670,7 +43029,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>6</v>
@@ -42742,10 +43101,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>6</v>
@@ -43915,10 +44274,10 @@
         <v>6</v>
       </c>
       <c r="R18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S18" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="T18" s="14" t="s">
         <v>2</v>
@@ -43990,7 +44349,7 @@
         <v>6</v>
       </c>
       <c r="R19" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="S19" s="14" t="s">
         <v>5</v>
@@ -44290,12 +44649,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="42" priority="2">
+    <cfRule type="expression" dxfId="43" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="41" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>